<commit_message>
Conduits prevent spawning of drowned
</commit_message>
<xml_diff>
--- a/Server Mod List.xlsx
+++ b/Server Mod List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Documents\My Documents\Lads-Modded-Minecraft-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB81FC8-E8F5-471B-BA3F-A19B3D2A00EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56091F26-A1BB-49B9-A7C3-17E1AA03D2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{55D671F0-0FE6-417B-B157-61E7F92E80E9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{55D671F0-0FE6-417B-B157-61E7F92E80E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="279">
   <si>
     <t>Mod Name</t>
   </si>
@@ -889,6 +889,15 @@
   </si>
   <si>
     <t>Improves advancement screen readability</t>
+  </si>
+  <si>
+    <t>Conduits Prevent Drowned</t>
+  </si>
+  <si>
+    <t>Conduits prevent spawning of drowned within range</t>
+  </si>
+  <si>
+    <t>Tweaks</t>
   </si>
 </sst>
 </file>
@@ -1546,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73755EB-73C1-4710-BFA9-A8996EFD459F}">
-  <dimension ref="B1:C148"/>
+  <dimension ref="B1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97:B99"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B147" sqref="B147:C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2380,22 +2389,49 @@
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B147" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C147" s="11" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B148" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="C147" s="11" t="s">
+      <c r="C148" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="148" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="14" t="s">
+    <row r="149" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B149" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="C148" s="15" t="s">
+      <c r="C149" s="15" t="s">
         <v>213</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B73:C73"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B118:C118"/>
     <mergeCell ref="B115:C115"/>
@@ -2412,25 +2448,6 @@
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2438,10 +2455,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA6AE23-A016-4677-B7E3-2CD8F0CC3272}">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3549,25 +3566,25 @@
       </c>
     </row>
     <row r="65" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="3" t="s">
-        <v>10</v>
+      <c r="B65" s="2" t="s">
+        <v>276</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>278</v>
       </c>
       <c r="D65" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F65" t="s">
-        <v>103</v>
+        <v>277</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C66" t="s">
         <v>72</v>
@@ -3576,15 +3593,15 @@
         <v>25</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F66" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C67" t="s">
         <v>72</v>
@@ -3593,32 +3610,32 @@
         <v>25</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F67" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="C68" t="s">
         <v>72</v>
       </c>
       <c r="D68" t="s">
-        <v>27</v>
-      </c>
-      <c r="E68" t="s">
-        <v>87</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>198</v>
+        <v>25</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F68" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C69" t="s">
         <v>72</v>
@@ -3627,7 +3644,7 @@
         <v>27</v>
       </c>
       <c r="E69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>198</v>
@@ -3635,7 +3652,7 @@
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C70" t="s">
         <v>72</v>
@@ -3644,7 +3661,7 @@
         <v>27</v>
       </c>
       <c r="E70" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>198</v>
@@ -3652,7 +3669,7 @@
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C71" t="s">
         <v>72</v>
@@ -3661,7 +3678,7 @@
         <v>27</v>
       </c>
       <c r="E71" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>198</v>
@@ -3669,7 +3686,7 @@
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C72" t="s">
         <v>72</v>
@@ -3678,7 +3695,7 @@
         <v>27</v>
       </c>
       <c r="E72" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>198</v>
@@ -3686,7 +3703,7 @@
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="3" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C73" t="s">
         <v>72</v>
@@ -3695,7 +3712,7 @@
         <v>27</v>
       </c>
       <c r="E73" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>198</v>
@@ -3703,7 +3720,7 @@
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C74" t="s">
         <v>72</v>
@@ -3712,7 +3729,7 @@
         <v>27</v>
       </c>
       <c r="E74" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>198</v>
@@ -3720,7 +3737,7 @@
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C75" t="s">
         <v>72</v>
@@ -3729,7 +3746,7 @@
         <v>27</v>
       </c>
       <c r="E75" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>198</v>
@@ -3737,7 +3754,7 @@
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="C76" t="s">
         <v>72</v>
@@ -3745,8 +3762,8 @@
       <c r="D76" t="s">
         <v>27</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>183</v>
+      <c r="E76" t="s">
+        <v>142</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>198</v>
@@ -3754,7 +3771,7 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C77" t="s">
         <v>72</v>
@@ -3763,7 +3780,7 @@
         <v>27</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>198</v>
@@ -3771,7 +3788,7 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C78" t="s">
         <v>72</v>
@@ -3780,7 +3797,7 @@
         <v>27</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>198</v>
@@ -3788,7 +3805,7 @@
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C79" t="s">
         <v>72</v>
@@ -3797,7 +3814,7 @@
         <v>27</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>198</v>
@@ -3805,7 +3822,7 @@
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C80" t="s">
         <v>72</v>
@@ -3814,7 +3831,7 @@
         <v>27</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>198</v>
@@ -3822,7 +3839,7 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C81" t="s">
         <v>72</v>
@@ -3831,7 +3848,7 @@
         <v>27</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>198</v>
@@ -3839,7 +3856,7 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B82" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C82" t="s">
         <v>72</v>
@@ -3848,7 +3865,7 @@
         <v>27</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>198</v>
@@ -3856,7 +3873,7 @@
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" s="3" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="C83" t="s">
         <v>72</v>
@@ -3865,7 +3882,7 @@
         <v>27</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>198</v>
@@ -3873,7 +3890,7 @@
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B84" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C84" t="s">
         <v>72</v>
@@ -3882,7 +3899,7 @@
         <v>27</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>198</v>
@@ -3890,7 +3907,7 @@
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C85" t="s">
         <v>72</v>
@@ -3899,7 +3916,7 @@
         <v>27</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>198</v>
@@ -3907,7 +3924,7 @@
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
-        <v>274</v>
+        <v>215</v>
       </c>
       <c r="C86" t="s">
         <v>72</v>
@@ -3916,24 +3933,24 @@
         <v>27</v>
       </c>
       <c r="E86" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B87" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C87" t="s">
+        <v>72</v>
+      </c>
+      <c r="D87" t="s">
+        <v>27</v>
+      </c>
+      <c r="E87" s="5" t="s">
         <v>275</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B87" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" t="s">
-        <v>64</v>
-      </c>
-      <c r="D87" t="s">
-        <v>27</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>198</v>
@@ -3941,7 +3958,7 @@
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C88" t="s">
         <v>64</v>
@@ -3950,7 +3967,7 @@
         <v>27</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F88" s="5" t="s">
         <v>198</v>
@@ -3958,7 +3975,7 @@
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="C89" t="s">
         <v>64</v>
@@ -3966,8 +3983,8 @@
       <c r="D89" t="s">
         <v>27</v>
       </c>
-      <c r="E89" t="s">
-        <v>86</v>
+      <c r="E89" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>198</v>
@@ -3975,7 +3992,7 @@
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="C90" t="s">
         <v>64</v>
@@ -3984,7 +4001,7 @@
         <v>27</v>
       </c>
       <c r="E90" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>198</v>
@@ -3992,7 +4009,7 @@
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C91" t="s">
         <v>64</v>
@@ -4001,7 +4018,7 @@
         <v>27</v>
       </c>
       <c r="E91" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>198</v>
@@ -4009,7 +4026,7 @@
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C92" t="s">
         <v>64</v>
@@ -4018,7 +4035,7 @@
         <v>27</v>
       </c>
       <c r="E92" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>198</v>
@@ -4026,41 +4043,58 @@
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B93" s="2" t="s">
-        <v>176</v>
+        <v>123</v>
       </c>
       <c r="C93" t="s">
         <v>64</v>
       </c>
       <c r="D93" t="s">
-        <v>25</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="F93" t="s">
-        <v>177</v>
+        <v>27</v>
+      </c>
+      <c r="E93" t="s">
+        <v>143</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B94" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C94" t="s">
         <v>64</v>
       </c>
       <c r="D94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E94" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F94" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B95" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C95" t="s">
+        <v>64</v>
+      </c>
+      <c r="D95" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="F94" s="5" t="s">
+      <c r="F95" s="5" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F94">
-    <sortCondition ref="C94"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F95">
+    <sortCondition ref="C95"/>
   </sortState>
   <conditionalFormatting sqref="F24 F31 E47">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">

</xml_diff>

<commit_message>
Better FPS mod that improves chunk rendering
</commit_message>
<xml_diff>
--- a/Server Mod List.xlsx
+++ b/Server Mod List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Documents\My Documents\Lads-Modded-Minecraft-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56091F26-A1BB-49B9-A7C3-17E1AA03D2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF0C90B-0EED-4476-8727-77305E75CF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{55D671F0-0FE6-417B-B157-61E7F92E80E9}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="280">
   <si>
     <t>Mod Name</t>
   </si>
@@ -898,6 +898,9 @@
   </si>
   <si>
     <t>Tweaks</t>
+  </si>
+  <si>
+    <t>Better FPS</t>
   </si>
 </sst>
 </file>
@@ -2413,25 +2416,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B73:C73"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B118:C118"/>
     <mergeCell ref="B115:C115"/>
@@ -2448,6 +2432,25 @@
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2455,10 +2458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA6AE23-A016-4677-B7E3-2CD8F0CC3272}">
-  <dimension ref="A1:M95"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3209,59 +3212,59 @@
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C44" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="C44" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" t="s">
-        <v>91</v>
-      </c>
-      <c r="F44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="C45" t="s">
         <v>61</v>
       </c>
       <c r="D45" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E45" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>198</v>
+        <v>91</v>
+      </c>
+      <c r="F45" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
         <v>61</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="8" t="s">
-        <v>80</v>
+      <c r="B47" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="C47" t="s">
         <v>61</v>
@@ -3270,15 +3273,15 @@
         <v>27</v>
       </c>
       <c r="E47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="2" t="s">
-        <v>82</v>
+      <c r="B48" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="C48" t="s">
         <v>61</v>
@@ -3287,7 +3290,7 @@
         <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>198</v>
@@ -3295,16 +3298,16 @@
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s">
         <v>61</v>
       </c>
       <c r="D49" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>198</v>
@@ -3312,16 +3315,16 @@
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
         <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E50" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>198</v>
@@ -3329,75 +3332,75 @@
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" t="s">
+        <v>85</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="C51" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B52" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C52" t="s">
         <v>60</v>
       </c>
       <c r="D52" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F52" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C53" t="s">
         <v>60</v>
       </c>
       <c r="D53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>198</v>
+        <v>58</v>
+      </c>
+      <c r="F53" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C54" t="s">
-        <v>223</v>
-      </c>
-      <c r="D54" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" t="s">
-        <v>140</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B55" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="C55" t="s">
         <v>223</v>
@@ -3405,16 +3408,16 @@
       <c r="D55" t="s">
         <v>27</v>
       </c>
-      <c r="E55" s="5" t="s">
-        <v>190</v>
+      <c r="E55" t="s">
+        <v>140</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B56" s="2" t="s">
-        <v>124</v>
+      <c r="B56" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="C56" t="s">
         <v>223</v>
@@ -3422,8 +3425,8 @@
       <c r="D56" t="s">
         <v>27</v>
       </c>
-      <c r="E56" t="s">
-        <v>144</v>
+      <c r="E56" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>198</v>
@@ -3431,7 +3434,7 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C57" t="s">
         <v>223</v>
@@ -3440,7 +3443,7 @@
         <v>27</v>
       </c>
       <c r="E57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>198</v>
@@ -3448,7 +3451,7 @@
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C58" t="s">
         <v>223</v>
@@ -3457,7 +3460,7 @@
         <v>27</v>
       </c>
       <c r="E58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>198</v>
@@ -3465,7 +3468,7 @@
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C59" t="s">
         <v>223</v>
@@ -3474,7 +3477,7 @@
         <v>27</v>
       </c>
       <c r="E59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>198</v>
@@ -3482,7 +3485,7 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="C60" t="s">
         <v>223</v>
@@ -3490,16 +3493,16 @@
       <c r="D60" t="s">
         <v>27</v>
       </c>
-      <c r="E60" s="5" t="s">
-        <v>157</v>
+      <c r="E60" t="s">
+        <v>147</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B61" s="7" t="s">
-        <v>159</v>
+      <c r="B61" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="C61" t="s">
         <v>223</v>
@@ -3508,7 +3511,7 @@
         <v>27</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>198</v>
@@ -3516,7 +3519,7 @@
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="7" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C62" t="s">
         <v>223</v>
@@ -3525,7 +3528,7 @@
         <v>27</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>198</v>
@@ -3533,7 +3536,7 @@
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C63" t="s">
         <v>223</v>
@@ -3542,15 +3545,15 @@
         <v>27</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B64" s="2" t="s">
-        <v>212</v>
+      <c r="B64" s="7" t="s">
+        <v>169</v>
       </c>
       <c r="C64" t="s">
         <v>223</v>
@@ -3559,7 +3562,7 @@
         <v>27</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>198</v>
@@ -3567,41 +3570,41 @@
     </row>
     <row r="65" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C65" t="s">
+        <v>223</v>
+      </c>
+      <c r="D65" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B66" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>278</v>
       </c>
-      <c r="D65" t="s">
-        <v>27</v>
-      </c>
-      <c r="E65" s="5" t="s">
+      <c r="D66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="F65" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B66" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C66" t="s">
-        <v>72</v>
-      </c>
-      <c r="D66" t="s">
-        <v>25</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F66" t="s">
-        <v>103</v>
+      <c r="F66" s="5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C67" t="s">
         <v>72</v>
@@ -3610,15 +3613,15 @@
         <v>25</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F67" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C68" t="s">
         <v>72</v>
@@ -3627,32 +3630,32 @@
         <v>25</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="C69" t="s">
         <v>72</v>
       </c>
       <c r="D69" t="s">
-        <v>27</v>
-      </c>
-      <c r="E69" t="s">
-        <v>87</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>198</v>
+        <v>25</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F69" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C70" t="s">
         <v>72</v>
@@ -3661,7 +3664,7 @@
         <v>27</v>
       </c>
       <c r="E70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>198</v>
@@ -3669,7 +3672,7 @@
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C71" t="s">
         <v>72</v>
@@ -3678,7 +3681,7 @@
         <v>27</v>
       </c>
       <c r="E71" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>198</v>
@@ -3686,7 +3689,7 @@
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C72" t="s">
         <v>72</v>
@@ -3695,7 +3698,7 @@
         <v>27</v>
       </c>
       <c r="E72" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>198</v>
@@ -3703,7 +3706,7 @@
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C73" t="s">
         <v>72</v>
@@ -3712,7 +3715,7 @@
         <v>27</v>
       </c>
       <c r="E73" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>198</v>
@@ -3720,7 +3723,7 @@
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C74" t="s">
         <v>72</v>
@@ -3729,7 +3732,7 @@
         <v>27</v>
       </c>
       <c r="E74" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>198</v>
@@ -3737,7 +3740,7 @@
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="3" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C75" t="s">
         <v>72</v>
@@ -3746,7 +3749,7 @@
         <v>27</v>
       </c>
       <c r="E75" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>198</v>
@@ -3754,7 +3757,7 @@
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C76" t="s">
         <v>72</v>
@@ -3763,7 +3766,7 @@
         <v>27</v>
       </c>
       <c r="E76" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>198</v>
@@ -3771,7 +3774,7 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="C77" t="s">
         <v>72</v>
@@ -3779,8 +3782,8 @@
       <c r="D77" t="s">
         <v>27</v>
       </c>
-      <c r="E77" s="5" t="s">
-        <v>183</v>
+      <c r="E77" t="s">
+        <v>142</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>198</v>
@@ -3788,7 +3791,7 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C78" t="s">
         <v>72</v>
@@ -3797,7 +3800,7 @@
         <v>27</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>198</v>
@@ -3805,7 +3808,7 @@
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C79" t="s">
         <v>72</v>
@@ -3814,7 +3817,7 @@
         <v>27</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>198</v>
@@ -3822,7 +3825,7 @@
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C80" t="s">
         <v>72</v>
@@ -3831,7 +3834,7 @@
         <v>27</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>198</v>
@@ -3839,7 +3842,7 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C81" t="s">
         <v>72</v>
@@ -3848,7 +3851,7 @@
         <v>27</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>198</v>
@@ -3856,7 +3859,7 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B82" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C82" t="s">
         <v>72</v>
@@ -3865,7 +3868,7 @@
         <v>27</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>198</v>
@@ -3873,7 +3876,7 @@
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C83" t="s">
         <v>72</v>
@@ -3882,7 +3885,7 @@
         <v>27</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>198</v>
@@ -3890,7 +3893,7 @@
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B84" s="3" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="C84" t="s">
         <v>72</v>
@@ -3899,7 +3902,7 @@
         <v>27</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>198</v>
@@ -3907,7 +3910,7 @@
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C85" t="s">
         <v>72</v>
@@ -3916,7 +3919,7 @@
         <v>27</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>198</v>
@@ -3924,7 +3927,7 @@
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C86" t="s">
         <v>72</v>
@@ -3933,7 +3936,7 @@
         <v>27</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>198</v>
@@ -3941,7 +3944,7 @@
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
-        <v>274</v>
+        <v>215</v>
       </c>
       <c r="C87" t="s">
         <v>72</v>
@@ -3950,24 +3953,24 @@
         <v>27</v>
       </c>
       <c r="E87" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B88" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C88" t="s">
+        <v>72</v>
+      </c>
+      <c r="D88" t="s">
+        <v>27</v>
+      </c>
+      <c r="E88" s="5" t="s">
         <v>275</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B88" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C88" t="s">
-        <v>64</v>
-      </c>
-      <c r="D88" t="s">
-        <v>27</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="F88" s="5" t="s">
         <v>198</v>
@@ -3975,7 +3978,7 @@
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C89" t="s">
         <v>64</v>
@@ -3984,7 +3987,7 @@
         <v>27</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>198</v>
@@ -3992,7 +3995,7 @@
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="C90" t="s">
         <v>64</v>
@@ -4000,8 +4003,8 @@
       <c r="D90" t="s">
         <v>27</v>
       </c>
-      <c r="E90" t="s">
-        <v>86</v>
+      <c r="E90" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>198</v>
@@ -4009,7 +4012,7 @@
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="C91" t="s">
         <v>64</v>
@@ -4018,7 +4021,7 @@
         <v>27</v>
       </c>
       <c r="E91" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>198</v>
@@ -4026,7 +4029,7 @@
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C92" t="s">
         <v>64</v>
@@ -4035,7 +4038,7 @@
         <v>27</v>
       </c>
       <c r="E92" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>198</v>
@@ -4043,7 +4046,7 @@
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B93" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C93" t="s">
         <v>64</v>
@@ -4052,7 +4055,7 @@
         <v>27</v>
       </c>
       <c r="E93" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>198</v>
@@ -4060,41 +4063,58 @@
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B94" s="2" t="s">
-        <v>176</v>
+        <v>123</v>
       </c>
       <c r="C94" t="s">
         <v>64</v>
       </c>
       <c r="D94" t="s">
-        <v>25</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="F94" t="s">
-        <v>177</v>
+        <v>27</v>
+      </c>
+      <c r="E94" t="s">
+        <v>143</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C95" t="s">
         <v>64</v>
       </c>
       <c r="D95" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E95" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F95" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B96" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C96" t="s">
+        <v>64</v>
+      </c>
+      <c r="D96" t="s">
+        <v>27</v>
+      </c>
+      <c r="E96" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="F95" s="5" t="s">
+      <c r="F96" s="5" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F95">
-    <sortCondition ref="C95"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F96">
+    <sortCondition ref="C96"/>
   </sortState>
   <conditionalFormatting sqref="F24 F31 E47">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">

</xml_diff>